<commit_message>
update 74hc595.c/74hc595.h new gpio.cpp/h
Signed-off-by: hu_zhihao <hu_zhihao@sina.cn>
</commit_message>
<xml_diff>
--- a/Doc/IO信息.xlsx
+++ b/Doc/IO信息.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5970" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,6 +287,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -296,6 +300,10 @@
   </si>
   <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -343,7 +351,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,6 +367,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,31 +472,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -490,6 +492,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,13 +1205,13 @@
   <dimension ref="B4:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.125" customWidth="1"/>
+    <col min="6" max="7" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1196,10 +1224,10 @@
       <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1211,532 +1239,532 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C5" s="13"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="14">
         <v>1</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="17">
         <v>2</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="6"/>
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="15">
+        <v>3</v>
+      </c>
+      <c r="G6" s="18">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3</v>
+      </c>
+      <c r="F7" s="15">
+        <v>5</v>
+      </c>
+      <c r="G7" s="18">
+        <v>6</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5">
+        <v>4</v>
+      </c>
+      <c r="F8" s="15">
+        <v>7</v>
+      </c>
+      <c r="G8" s="18">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="15">
+        <v>9</v>
+      </c>
+      <c r="G9" s="18">
+        <v>10</v>
+      </c>
+      <c r="H9" s="5">
+        <v>15</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="5">
+        <v>17</v>
+      </c>
+      <c r="F10" s="15">
+        <v>11</v>
+      </c>
+      <c r="G10" s="18">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5">
+        <v>18</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5">
+        <v>27</v>
+      </c>
+      <c r="F11" s="15">
+        <v>13</v>
+      </c>
+      <c r="G11" s="18">
+        <v>14</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5">
+        <v>22</v>
+      </c>
+      <c r="F12" s="15">
+        <v>15</v>
+      </c>
+      <c r="G12" s="18">
+        <v>16</v>
+      </c>
+      <c r="H12" s="5">
         <v>23</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="11">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6">
-        <v>3</v>
-      </c>
-      <c r="G6" s="7">
-        <v>4</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="I12" s="4"/>
+      <c r="J12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="F13" s="15">
+        <v>17</v>
+      </c>
+      <c r="G13" s="18">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5">
+        <v>24</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="5">
+        <v>10</v>
+      </c>
+      <c r="F14" s="15">
+        <v>19</v>
+      </c>
+      <c r="G14" s="18">
+        <v>20</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="5">
+        <v>9</v>
+      </c>
+      <c r="F15" s="15">
+        <v>21</v>
+      </c>
+      <c r="G15" s="18">
+        <v>22</v>
+      </c>
+      <c r="H15" s="5">
+        <v>25</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="5">
+        <v>11</v>
+      </c>
+      <c r="F16" s="15">
+        <v>23</v>
+      </c>
+      <c r="G16" s="18">
+        <v>24</v>
+      </c>
+      <c r="H16" s="5">
+        <v>8</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="15">
+        <v>25</v>
+      </c>
+      <c r="G17" s="18">
+        <v>26</v>
+      </c>
+      <c r="H17" s="5">
+        <v>7</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="15">
+        <v>27</v>
+      </c>
+      <c r="G18" s="18">
+        <v>28</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5">
+        <v>5</v>
+      </c>
+      <c r="F19" s="15">
+        <v>29</v>
+      </c>
+      <c r="G19" s="18">
+        <v>30</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5">
+        <v>6</v>
+      </c>
+      <c r="F20" s="15">
+        <v>31</v>
+      </c>
+      <c r="G20" s="18">
+        <v>32</v>
+      </c>
+      <c r="H20" s="5">
+        <v>12</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5">
+        <v>13</v>
+      </c>
+      <c r="F21" s="15">
+        <v>33</v>
+      </c>
+      <c r="G21" s="18">
+        <v>34</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="5">
+        <v>19</v>
+      </c>
+      <c r="F22" s="15">
+        <v>35</v>
+      </c>
+      <c r="G22" s="18">
+        <v>36</v>
+      </c>
+      <c r="H22" s="5">
+        <v>16</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5">
+        <v>26</v>
+      </c>
+      <c r="F23" s="15">
+        <v>37</v>
+      </c>
+      <c r="G23" s="18">
+        <v>38</v>
+      </c>
+      <c r="H23" s="5">
+        <v>20</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="16">
+        <v>39</v>
+      </c>
+      <c r="G24" s="19">
         <v>40</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="11">
-        <v>3</v>
-      </c>
-      <c r="F7" s="6">
-        <v>5</v>
-      </c>
-      <c r="G7" s="7">
-        <v>6</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11">
-        <v>4</v>
-      </c>
-      <c r="F8" s="6">
-        <v>7</v>
-      </c>
-      <c r="G8" s="7">
-        <v>8</v>
-      </c>
-      <c r="H8" s="11">
-        <v>14</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="6">
-        <v>9</v>
-      </c>
-      <c r="G9" s="7">
-        <v>10</v>
-      </c>
-      <c r="H9" s="11">
-        <v>15</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="11">
-        <v>17</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="H24" s="5">
+        <v>21</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="7">
-        <v>12</v>
-      </c>
-      <c r="H10" s="11">
-        <v>18</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11">
-        <v>27</v>
-      </c>
-      <c r="F11" s="6">
-        <v>13</v>
-      </c>
-      <c r="G11" s="7">
-        <v>14</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11">
-        <v>22</v>
-      </c>
-      <c r="F12" s="6">
-        <v>15</v>
-      </c>
-      <c r="G12" s="7">
-        <v>16</v>
-      </c>
-      <c r="H12" s="11">
-        <v>23</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="6">
-        <v>17</v>
-      </c>
-      <c r="G13" s="7">
-        <v>18</v>
-      </c>
-      <c r="H13" s="11">
-        <v>24</v>
-      </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="11">
-        <v>10</v>
-      </c>
-      <c r="F14" s="6">
-        <v>19</v>
-      </c>
-      <c r="G14" s="7">
-        <v>20</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="11">
-        <v>9</v>
-      </c>
-      <c r="F15" s="6">
-        <v>21</v>
-      </c>
-      <c r="G15" s="7">
-        <v>22</v>
-      </c>
-      <c r="H15" s="11">
-        <v>25</v>
-      </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="11">
-        <v>11</v>
-      </c>
-      <c r="F16" s="6">
-        <v>23</v>
-      </c>
-      <c r="G16" s="7">
-        <v>24</v>
-      </c>
-      <c r="H16" s="11">
-        <v>8</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="6">
-        <v>25</v>
-      </c>
-      <c r="G17" s="7">
-        <v>26</v>
-      </c>
-      <c r="H17" s="11">
-        <v>7</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="11">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6">
-        <v>27</v>
-      </c>
-      <c r="G18" s="7">
-        <v>28</v>
-      </c>
-      <c r="H18" s="11">
-        <v>1</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11">
-        <v>5</v>
-      </c>
-      <c r="F19" s="6">
-        <v>29</v>
-      </c>
-      <c r="G19" s="7">
-        <v>30</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11">
-        <v>6</v>
-      </c>
-      <c r="F20" s="6">
-        <v>31</v>
-      </c>
-      <c r="G20" s="7">
-        <v>32</v>
-      </c>
-      <c r="H20" s="11">
-        <v>12</v>
-      </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B21" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11">
-        <v>13</v>
-      </c>
-      <c r="F21" s="6">
-        <v>33</v>
-      </c>
-      <c r="G21" s="7">
-        <v>34</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="11">
-        <v>19</v>
-      </c>
-      <c r="F22" s="6">
-        <v>35</v>
-      </c>
-      <c r="G22" s="7">
-        <v>36</v>
-      </c>
-      <c r="H22" s="11">
-        <v>16</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11">
-        <v>26</v>
-      </c>
-      <c r="F23" s="6">
-        <v>37</v>
-      </c>
-      <c r="G23" s="7">
-        <v>38</v>
-      </c>
-      <c r="H23" s="11">
-        <v>20</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="8">
-        <v>39</v>
-      </c>
-      <c r="G24" s="9">
-        <v>40</v>
-      </c>
-      <c r="H24" s="11">
-        <v>21</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>77</v>
+      <c r="K24" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>